<commit_message>
Cập nhật cách tính tye lệ pixel: Lấy tỷ lệ pixel tại chính khoảng mà điểm laser nằm
</commit_message>
<xml_diff>
--- a/Evaluation Results/video13-6.xlsx
+++ b/Evaluation Results/video13-6.xlsx
@@ -367,18 +367,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>3.34</v>
+        <v>3.36</v>
       </c>
       <c r="B2">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>3.38</v>
+        <v>3.39</v>
       </c>
       <c r="B3">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -391,7 +391,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>3.33</v>
+        <v>3.34</v>
       </c>
       <c r="B5">
         <v>-0.1</v>
@@ -399,7 +399,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>3.39</v>
+        <v>3.42</v>
       </c>
       <c r="B6">
         <v>-0.12</v>
@@ -407,10 +407,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>3.44</v>
+        <v>3.45</v>
       </c>
       <c r="B7">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -418,15 +418,15 @@
         <v>3.49</v>
       </c>
       <c r="B8">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>3.58</v>
+        <v>3.6</v>
       </c>
       <c r="B9">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -434,12 +434,12 @@
         <v>3.56</v>
       </c>
       <c r="B10">
-        <v>-0.11</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>3.6</v>
+        <v>3.59</v>
       </c>
       <c r="B11">
         <v>-0.04</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>3.62</v>
+        <v>3.64</v>
       </c>
       <c r="B13">
         <v>-0.01</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>3.7</v>
+        <v>3.71</v>
       </c>
       <c r="B15">
         <v>-0.04</v>
@@ -479,15 +479,15 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>3.7</v>
+        <v>3.71</v>
       </c>
       <c r="B16">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>3.58</v>
+        <v>3.59</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -506,20 +506,20 @@
         <v>3.68</v>
       </c>
       <c r="B19">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>3.72</v>
+        <v>3.73</v>
       </c>
       <c r="B20">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>3.74</v>
+        <v>3.78</v>
       </c>
       <c r="B21">
         <v>0.02</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>3.66</v>
+        <v>3.68</v>
       </c>
       <c r="B22">
         <v>-0.04</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>3.66</v>
+        <v>3.68</v>
       </c>
       <c r="B23">
         <v>-0.04</v>
@@ -543,10 +543,10 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>3.74</v>
+        <v>3.75</v>
       </c>
       <c r="B24">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -554,20 +554,20 @@
         <v>3.79</v>
       </c>
       <c r="B25">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>3.81</v>
+        <v>3.82</v>
       </c>
       <c r="B26">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>3.81</v>
+        <v>3.88</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -575,23 +575,23 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>3.89</v>
+        <v>3.93</v>
       </c>
       <c r="B28">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>3.9</v>
+        <v>3.91</v>
       </c>
       <c r="B29">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>3.86</v>
+        <v>3.93</v>
       </c>
       <c r="B30">
         <v>-0.02</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>3.9</v>
+        <v>3.92</v>
       </c>
       <c r="B31">
         <v>-0.01</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>4.2</v>
+        <v>4.21</v>
       </c>
       <c r="B35">
         <v>-0.02</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>4.2</v>
+        <v>4.21</v>
       </c>
       <c r="B36">
         <v>0.04</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>4.16</v>
+        <v>4.17</v>
       </c>
       <c r="B37">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -674,7 +674,7 @@
         <v>4.27</v>
       </c>
       <c r="B40">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -682,7 +682,7 @@
         <v>4.23</v>
       </c>
       <c r="B41">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -698,12 +698,12 @@
         <v>4.29</v>
       </c>
       <c r="B43">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>4.3</v>
+        <v>4.31</v>
       </c>
       <c r="B44">
         <v>-0.04</v>
@@ -711,23 +711,23 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>4.28</v>
+        <v>4.29</v>
       </c>
       <c r="B45">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>4.29</v>
+        <v>4.3</v>
       </c>
       <c r="B46">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>4.29</v>
+        <v>4.31</v>
       </c>
       <c r="B47">
         <v>-0.03</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>4.29</v>
+        <v>4.31</v>
       </c>
       <c r="B48">
         <v>-0.01</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>4.32</v>
+        <v>4.33</v>
       </c>
       <c r="B49">
         <v>-0.04</v>
@@ -786,12 +786,12 @@
         <v>4.24</v>
       </c>
       <c r="B54">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55">
-        <v>4.15</v>
+        <v>4.16</v>
       </c>
       <c r="B55">
         <v>-0.04</v>
@@ -834,7 +834,7 @@
         <v>4.05</v>
       </c>
       <c r="B60">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -855,7 +855,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63">
-        <v>3.91</v>
+        <v>3.95</v>
       </c>
       <c r="B63">
         <v>0.02</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64">
-        <v>3.91</v>
+        <v>3.99</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65">
-        <v>3.85</v>
+        <v>3.87</v>
       </c>
       <c r="B65">
         <v>0.1</v>
@@ -879,15 +879,15 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66">
-        <v>3.8</v>
+        <v>3.85</v>
       </c>
       <c r="B66">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67">
-        <v>3.72</v>
+        <v>3.75</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -895,10 +895,10 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68">
-        <v>3.71</v>
+        <v>3.72</v>
       </c>
       <c r="B68">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -906,20 +906,20 @@
         <v>3.65</v>
       </c>
       <c r="B69">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70">
-        <v>3.63</v>
+        <v>3.64</v>
       </c>
       <c r="B70">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71">
-        <v>3.61</v>
+        <v>3.62</v>
       </c>
       <c r="B71">
         <v>0.03</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72">
-        <v>3.49</v>
+        <v>3.5</v>
       </c>
       <c r="B72">
         <v>0.03</v>
@@ -935,10 +935,10 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73">
-        <v>3.47</v>
+        <v>3.48</v>
       </c>
       <c r="B73">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -946,12 +946,12 @@
         <v>3.37</v>
       </c>
       <c r="B74">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75">
-        <v>3.46</v>
+        <v>3.48</v>
       </c>
       <c r="B75">
         <v>-0.04</v>
@@ -959,10 +959,10 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76">
-        <v>3.51</v>
+        <v>3.52</v>
       </c>
       <c r="B76">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -970,20 +970,20 @@
         <v>3.47</v>
       </c>
       <c r="B77">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78">
-        <v>3.44</v>
+        <v>3.45</v>
       </c>
       <c r="B78">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79">
-        <v>3.29</v>
+        <v>3.31</v>
       </c>
       <c r="B79">
         <v>-0.04</v>
@@ -991,15 +991,15 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80">
-        <v>3.19</v>
+        <v>3.2</v>
       </c>
       <c r="B80">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81">
-        <v>3.15</v>
+        <v>3.16</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1010,7 +1010,7 @@
         <v>3.28</v>
       </c>
       <c r="B82">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>3.22</v>
       </c>
       <c r="B83">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1026,15 +1026,15 @@
         <v>3.15</v>
       </c>
       <c r="B84">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85">
-        <v>3.13</v>
+        <v>3.14</v>
       </c>
       <c r="B85">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>3.23</v>
       </c>
       <c r="B86">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>3.06</v>
       </c>
       <c r="B87">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1058,12 +1058,12 @@
         <v>3.08</v>
       </c>
       <c r="B88">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89">
-        <v>2.96</v>
+        <v>2.97</v>
       </c>
       <c r="B89">
         <v>-0.04</v>
@@ -1074,52 +1074,52 @@
         <v>3.03</v>
       </c>
       <c r="B90">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91">
-        <v>2.93</v>
+        <v>2.95</v>
       </c>
       <c r="B91">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92">
-        <v>2.9</v>
+        <v>2.92</v>
       </c>
       <c r="B92">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93">
-        <v>2.89</v>
+        <v>2.91</v>
       </c>
       <c r="B93">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94">
-        <v>2.82</v>
+        <v>2.86</v>
       </c>
       <c r="B94">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95">
-        <v>2.82</v>
+        <v>2.83</v>
       </c>
       <c r="B95">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96">
-        <v>2.7</v>
+        <v>2.73</v>
       </c>
       <c r="B96">
         <v>-0.1</v>
@@ -1130,87 +1130,87 @@
         <v>2.79</v>
       </c>
       <c r="B97">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98">
-        <v>2.7</v>
+        <v>2.71</v>
       </c>
       <c r="B98">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99">
-        <v>2.66</v>
+        <v>2.69</v>
       </c>
       <c r="B99">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100">
-        <v>2.61</v>
+        <v>2.62</v>
       </c>
       <c r="B100">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101">
-        <v>2.62</v>
+        <v>2.64</v>
       </c>
       <c r="B101">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102">
-        <v>2.61</v>
+        <v>2.62</v>
       </c>
       <c r="B102">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103">
-        <v>2.53</v>
+        <v>2.55</v>
       </c>
       <c r="B103">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104">
-        <v>2.52</v>
+        <v>2.55</v>
       </c>
       <c r="B104">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105">
-        <v>2.53</v>
+        <v>2.54</v>
       </c>
       <c r="B105">
-        <v>-0.27</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106">
-        <v>2.51</v>
+        <v>2.54</v>
       </c>
       <c r="B106">
-        <v>-0.28</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107">
-        <v>2.57</v>
+        <v>2.58</v>
       </c>
       <c r="B107">
-        <v>-0.27</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1218,31 +1218,31 @@
         <v>2.46</v>
       </c>
       <c r="B108">
-        <v>-0.28</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109">
-        <v>2.48</v>
+        <v>2.49</v>
       </c>
       <c r="B109">
-        <v>-0.26</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110">
-        <v>2.44</v>
+        <v>2.47</v>
       </c>
       <c r="B110">
-        <v>-0.28</v>
+        <v>-0.26</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111">
-        <v>2.39</v>
+        <v>2.4</v>
       </c>
       <c r="B111">
-        <v>-0.29</v>
+        <v>-0.27</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>2.41</v>
       </c>
       <c r="B112">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>2.33</v>
       </c>
       <c r="B113">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1266,39 +1266,39 @@
         <v>2.32</v>
       </c>
       <c r="B114">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115">
-        <v>2.36</v>
+        <v>2.35</v>
       </c>
       <c r="B115">
-        <v>-0.26</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116">
-        <v>2.29</v>
+        <v>2.28</v>
       </c>
       <c r="B116">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117">
-        <v>2.24</v>
+        <v>2.25</v>
       </c>
       <c r="B117">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118">
-        <v>2.34</v>
+        <v>2.35</v>
       </c>
       <c r="B118">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1306,31 +1306,31 @@
         <v>2.38</v>
       </c>
       <c r="B119">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120">
-        <v>2.39</v>
+        <v>2.41</v>
       </c>
       <c r="B120">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121">
-        <v>2.37</v>
+        <v>2.39</v>
       </c>
       <c r="B121">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122">
-        <v>2.29</v>
+        <v>2.32</v>
       </c>
       <c r="B122">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1338,47 +1338,47 @@
         <v>2.37</v>
       </c>
       <c r="B123">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124">
-        <v>2.37</v>
+        <v>2.38</v>
       </c>
       <c r="B124">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125">
-        <v>2.37</v>
+        <v>2.39</v>
       </c>
       <c r="B125">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126">
-        <v>2.44</v>
+        <v>2.47</v>
       </c>
       <c r="B126">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127">
-        <v>2.38</v>
+        <v>2.4</v>
       </c>
       <c r="B127">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
-        <v>2.37</v>
+        <v>2.39</v>
       </c>
       <c r="B128">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1386,15 +1386,15 @@
         <v>2.43</v>
       </c>
       <c r="B129">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130">
-        <v>2.43</v>
+        <v>2.42</v>
       </c>
       <c r="B130">
-        <v>-0.21</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1402,15 +1402,15 @@
         <v>2.42</v>
       </c>
       <c r="B131">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132">
-        <v>2.43</v>
+        <v>2.44</v>
       </c>
       <c r="B132">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1418,76 +1418,76 @@
         <v>2.47</v>
       </c>
       <c r="B133">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134">
-        <v>2.43</v>
+        <v>2.44</v>
       </c>
       <c r="B134">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135">
-        <v>2.44</v>
+        <v>2.47</v>
       </c>
       <c r="B135">
-        <v>-0.26</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136">
-        <v>2.48</v>
+        <v>2.49</v>
       </c>
       <c r="B136">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137">
-        <v>2.57</v>
+        <v>2.58</v>
       </c>
       <c r="B137">
-        <v>-0.18</v>
+        <v>-0.17</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138">
-        <v>2.58</v>
+        <v>2.6</v>
       </c>
       <c r="B138">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139">
-        <v>2.63</v>
+        <v>2.64</v>
       </c>
       <c r="B139">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140">
-        <v>2.61</v>
+        <v>2.62</v>
       </c>
       <c r="B140">
-        <v>-0.12</v>
+        <v>-0.11</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141">
-        <v>2.71</v>
+        <v>2.73</v>
       </c>
       <c r="B141">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142">
-        <v>2.67</v>
+        <v>2.69</v>
       </c>
       <c r="B142">
         <v>-0.1</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143">
-        <v>2.76</v>
+        <v>2.77</v>
       </c>
       <c r="B143">
         <v>-0.13</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144">
-        <v>2.82</v>
+        <v>2.83</v>
       </c>
       <c r="B144">
         <v>-0.13</v>
@@ -1514,12 +1514,12 @@
         <v>2.88</v>
       </c>
       <c r="B145">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146">
-        <v>2.88</v>
+        <v>2.87</v>
       </c>
       <c r="B146">
         <v>-0.1</v>
@@ -1527,15 +1527,15 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147">
-        <v>2.93</v>
+        <v>2.95</v>
       </c>
       <c r="B147">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148">
-        <v>2.98</v>
+        <v>2.99</v>
       </c>
       <c r="B148">
         <v>-0.13</v>
@@ -1554,7 +1554,7 @@
         <v>3.09</v>
       </c>
       <c r="B150">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1562,12 +1562,12 @@
         <v>3.13</v>
       </c>
       <c r="B151">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152">
-        <v>3.16</v>
+        <v>3.17</v>
       </c>
       <c r="B152">
         <v>-0.04</v>
@@ -1586,28 +1586,28 @@
         <v>3.36</v>
       </c>
       <c r="B154">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155">
-        <v>3.39</v>
+        <v>3.4</v>
       </c>
       <c r="B155">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156">
-        <v>3.52</v>
+        <v>3.53</v>
       </c>
       <c r="B156">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157">
-        <v>3.58</v>
+        <v>3.6</v>
       </c>
       <c r="B157">
         <v>-0.04</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158">
-        <v>3.62</v>
+        <v>3.64</v>
       </c>
       <c r="B158">
         <v>-0.04</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159">
-        <v>3.72</v>
+        <v>3.77</v>
       </c>
       <c r="B159">
         <v>-0.01</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160">
-        <v>3.76</v>
+        <v>3.77</v>
       </c>
       <c r="B160">
         <v>-0.02</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161">
-        <v>3.79</v>
+        <v>3.85</v>
       </c>
       <c r="B161">
         <v>0.03</v>
@@ -1647,18 +1647,18 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162">
-        <v>3.9</v>
+        <v>3.91</v>
       </c>
       <c r="B162">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163">
-        <v>3.94</v>
+        <v>3.99</v>
       </c>
       <c r="B163">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1682,12 +1682,12 @@
         <v>4.15</v>
       </c>
       <c r="B166">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167">
-        <v>4.29</v>
+        <v>4.3</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="168" spans="1:2">
       <c r="A168">
-        <v>4.36</v>
+        <v>4.37</v>
       </c>
       <c r="B168">
         <v>0.03</v>
@@ -1719,18 +1719,18 @@
     </row>
     <row r="171" spans="1:2">
       <c r="A171">
-        <v>4.48</v>
+        <v>4.51</v>
       </c>
       <c r="B171">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172">
-        <v>4.58</v>
+        <v>4.59</v>
       </c>
       <c r="B172">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1738,20 +1738,20 @@
         <v>4.61</v>
       </c>
       <c r="B173">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174">
-        <v>4.62</v>
+        <v>4.63</v>
       </c>
       <c r="B174">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175">
-        <v>4.76</v>
+        <v>4.77</v>
       </c>
       <c r="B175">
         <v>0.02</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="177" spans="1:2">
       <c r="A177">
-        <v>4.71</v>
+        <v>4.73</v>
       </c>
       <c r="B177">
         <v>0.04</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="178" spans="1:2">
       <c r="A178">
-        <v>4.76</v>
+        <v>4.77</v>
       </c>
       <c r="B178">
         <v>0.04</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="179" spans="1:2">
       <c r="A179">
-        <v>4.79</v>
+        <v>4.78</v>
       </c>
       <c r="B179">
         <v>0.03</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180">
-        <v>4.79</v>
+        <v>4.81</v>
       </c>
       <c r="B180">
         <v>0.1</v>
@@ -1799,7 +1799,7 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181">
-        <v>4.77</v>
+        <v>4.8</v>
       </c>
       <c r="B181">
         <v>0.01</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="182" spans="1:2">
       <c r="A182">
-        <v>4.84</v>
+        <v>4.85</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -1818,52 +1818,52 @@
         <v>4.89</v>
       </c>
       <c r="B183">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184">
-        <v>4.84</v>
+        <v>4.85</v>
       </c>
       <c r="B184">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185">
-        <v>4.89</v>
+        <v>4.9</v>
       </c>
       <c r="B185">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186">
-        <v>4.9</v>
+        <v>4.93</v>
       </c>
       <c r="B186">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187">
-        <v>4.9</v>
+        <v>4.95</v>
       </c>
       <c r="B187">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188">
-        <v>4.93</v>
+        <v>4.95</v>
       </c>
       <c r="B188">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189">
-        <v>4.89</v>
+        <v>4.9</v>
       </c>
       <c r="B189">
         <v>-0.12</v>
@@ -1871,18 +1871,18 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190">
-        <v>4.86</v>
+        <v>4.87</v>
       </c>
       <c r="B190">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191">
-        <v>4.88</v>
+        <v>4.9</v>
       </c>
       <c r="B191">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1890,20 +1890,20 @@
         <v>4.9</v>
       </c>
       <c r="B192">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193">
-        <v>4.89</v>
+        <v>4.91</v>
       </c>
       <c r="B193">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194">
-        <v>4.91</v>
+        <v>4.92</v>
       </c>
       <c r="B194">
         <v>-0.03</v>
@@ -1911,23 +1911,23 @@
     </row>
     <row r="195" spans="1:2">
       <c r="A195">
-        <v>4.9</v>
+        <v>4.91</v>
       </c>
       <c r="B195">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196">
-        <v>4.93</v>
+        <v>4.94</v>
       </c>
       <c r="B196">
-        <v>-0.11</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197">
-        <v>4.94</v>
+        <v>4.97</v>
       </c>
       <c r="B197">
         <v>-0.04</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="198" spans="1:2">
       <c r="A198">
-        <v>4.94</v>
+        <v>4.95</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="199" spans="1:2">
       <c r="A199">
-        <v>4.96</v>
+        <v>4.97</v>
       </c>
       <c r="B199">
         <v>-0.02</v>
@@ -1954,7 +1954,7 @@
         <v>4.96</v>
       </c>
       <c r="B200">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1970,7 +1970,7 @@
         <v>4.99</v>
       </c>
       <c r="B202">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -1978,7 +1978,7 @@
         <v>5.04</v>
       </c>
       <c r="B203">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2026,7 +2026,7 @@
         <v>5.03</v>
       </c>
       <c r="B209">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2063,15 +2063,15 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214">
-        <v>4.94</v>
+        <v>4.97</v>
       </c>
       <c r="B214">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215">
-        <v>4.94</v>
+        <v>4.95</v>
       </c>
       <c r="B215">
         <v>0.01</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="216" spans="1:2">
       <c r="A216">
-        <v>4.9</v>
+        <v>4.91</v>
       </c>
       <c r="B216">
         <v>0.04</v>
@@ -2095,7 +2095,7 @@
     </row>
     <row r="218" spans="1:2">
       <c r="A218">
-        <v>4.82</v>
+        <v>4.81</v>
       </c>
       <c r="B218">
         <v>0.13</v>
@@ -2103,15 +2103,15 @@
     </row>
     <row r="219" spans="1:2">
       <c r="A219">
-        <v>4.91</v>
+        <v>4.94</v>
       </c>
       <c r="B219">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220">
-        <v>4.89</v>
+        <v>4.91</v>
       </c>
       <c r="B220">
         <v>0.1</v>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="221" spans="1:2">
       <c r="A221">
-        <v>4.9</v>
+        <v>4.92</v>
       </c>
       <c r="B221">
         <v>0.1</v>
@@ -2127,18 +2127,18 @@
     </row>
     <row r="222" spans="1:2">
       <c r="A222">
-        <v>4.91</v>
+        <v>4.92</v>
       </c>
       <c r="B222">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223">
-        <v>4.93</v>
+        <v>4.95</v>
       </c>
       <c r="B223">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2151,7 +2151,7 @@
     </row>
     <row r="225" spans="1:2">
       <c r="A225">
-        <v>4.94</v>
+        <v>4.95</v>
       </c>
       <c r="B225">
         <v>0.02</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="226" spans="1:2">
       <c r="A226">
-        <v>4.95</v>
+        <v>4.96</v>
       </c>
       <c r="B226">
         <v>0.01</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="228" spans="1:2">
       <c r="A228">
-        <v>4.88</v>
+        <v>4.93</v>
       </c>
       <c r="B228">
         <v>0.03</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="229" spans="1:2">
       <c r="A229">
-        <v>4.86</v>
+        <v>4.88</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="230" spans="1:2">
       <c r="A230">
-        <v>4.89</v>
+        <v>4.9</v>
       </c>
       <c r="B230">
         <v>0.02</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="231" spans="1:2">
       <c r="A231">
-        <v>4.9</v>
+        <v>4.91</v>
       </c>
       <c r="B231">
         <v>-0.02</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="233" spans="1:2">
       <c r="A233">
-        <v>4.81</v>
+        <v>4.8</v>
       </c>
       <c r="B233">
         <v>0.03</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="234" spans="1:2">
       <c r="A234">
-        <v>4.8</v>
+        <v>4.81</v>
       </c>
       <c r="B234">
         <v>0.04</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="235" spans="1:2">
       <c r="A235">
-        <v>4.82</v>
+        <v>4.83</v>
       </c>
       <c r="B235">
         <v>-0.03</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="236" spans="1:2">
       <c r="A236">
-        <v>4.81</v>
+        <v>4.82</v>
       </c>
       <c r="B236">
         <v>0.04</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="238" spans="1:2">
       <c r="A238">
-        <v>4.75</v>
+        <v>4.78</v>
       </c>
       <c r="B238">
         <v>0.02</v>
@@ -2266,12 +2266,12 @@
         <v>4.76</v>
       </c>
       <c r="B239">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240">
-        <v>4.8</v>
+        <v>4.81</v>
       </c>
       <c r="B240">
         <v>0.03</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="242" spans="1:2">
       <c r="A242">
-        <v>4.76</v>
+        <v>4.77</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -2295,15 +2295,15 @@
     </row>
     <row r="243" spans="1:2">
       <c r="A243">
-        <v>4.75</v>
+        <v>4.76</v>
       </c>
       <c r="B243">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244">
-        <v>4.77</v>
+        <v>4.78</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="245" spans="1:2">
       <c r="A245">
-        <v>4.74</v>
+        <v>4.77</v>
       </c>
       <c r="B245">
         <v>-0.01</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="246" spans="1:2">
       <c r="A246">
-        <v>4.71</v>
+        <v>4.76</v>
       </c>
       <c r="B246">
         <v>-0.01</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="247" spans="1:2">
       <c r="A247">
-        <v>4.77</v>
+        <v>4.79</v>
       </c>
       <c r="B247">
         <v>-0.04</v>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="248" spans="1:2">
       <c r="A248">
-        <v>4.77</v>
+        <v>4.79</v>
       </c>
       <c r="B248">
         <v>-0.03</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="249" spans="1:2">
       <c r="A249">
-        <v>4.77</v>
+        <v>4.78</v>
       </c>
       <c r="B249">
         <v>-0.01</v>
@@ -2367,7 +2367,7 @@
     </row>
     <row r="252" spans="1:2">
       <c r="A252">
-        <v>4.77</v>
+        <v>4.78</v>
       </c>
       <c r="B252">
         <v>-0.02</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="254" spans="1:2">
       <c r="A254">
-        <v>4.8</v>
+        <v>4.81</v>
       </c>
       <c r="B254">
         <v>-0.02</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="255" spans="1:2">
       <c r="A255">
-        <v>4.76</v>
+        <v>4.78</v>
       </c>
       <c r="B255">
         <v>-0.03</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="256" spans="1:2">
       <c r="A256">
-        <v>4.77</v>
+        <v>4.79</v>
       </c>
       <c r="B256">
         <v>-0.03</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="257" spans="1:2">
       <c r="A257">
-        <v>4.71</v>
+        <v>4.72</v>
       </c>
       <c r="B257">
         <v>-0.03</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="258" spans="1:2">
       <c r="A258">
-        <v>4.75</v>
+        <v>4.77</v>
       </c>
       <c r="B258">
         <v>-0.04</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="259" spans="1:2">
       <c r="A259">
-        <v>4.71</v>
+        <v>4.73</v>
       </c>
       <c r="B259">
         <v>-0.01</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="260" spans="1:2">
       <c r="A260">
-        <v>4.67</v>
+        <v>4.69</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -2439,7 +2439,7 @@
     </row>
     <row r="261" spans="1:2">
       <c r="A261">
-        <v>4.72</v>
+        <v>4.71</v>
       </c>
       <c r="B261">
         <v>0.01</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="262" spans="1:2">
       <c r="A262">
-        <v>4.6</v>
+        <v>4.61</v>
       </c>
       <c r="B262">
         <v>0.01</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="263" spans="1:2">
       <c r="A263">
-        <v>4.51</v>
+        <v>4.53</v>
       </c>
       <c r="B263">
         <v>0.02</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="266" spans="1:2">
       <c r="A266">
-        <v>4.43</v>
+        <v>4.45</v>
       </c>
       <c r="B266">
         <v>0.03</v>
@@ -2490,7 +2490,7 @@
         <v>4.38</v>
       </c>
       <c r="B267">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2498,7 +2498,7 @@
         <v>4.33</v>
       </c>
       <c r="B268">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2514,7 +2514,7 @@
         <v>4.14</v>
       </c>
       <c r="B270">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2527,15 +2527,15 @@
     </row>
     <row r="272" spans="1:2">
       <c r="A272">
-        <v>3.9</v>
+        <v>3.95</v>
       </c>
       <c r="B272">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273">
-        <v>3.85</v>
+        <v>3.86</v>
       </c>
       <c r="B273">
         <v>0.01</v>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="274" spans="1:2">
       <c r="A274">
-        <v>3.77</v>
+        <v>3.8</v>
       </c>
       <c r="B274">
         <v>0.04</v>
@@ -2551,7 +2551,7 @@
     </row>
     <row r="275" spans="1:2">
       <c r="A275">
-        <v>3.74</v>
+        <v>3.75</v>
       </c>
       <c r="B275">
         <v>0.03</v>
@@ -2559,7 +2559,7 @@
     </row>
     <row r="276" spans="1:2">
       <c r="A276">
-        <v>3.58</v>
+        <v>3.59</v>
       </c>
       <c r="B276">
         <v>0.01</v>
@@ -2567,15 +2567,15 @@
     </row>
     <row r="277" spans="1:2">
       <c r="A277">
-        <v>3.53</v>
+        <v>3.54</v>
       </c>
       <c r="B277">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278">
-        <v>3.25</v>
+        <v>3.26</v>
       </c>
       <c r="B278">
         <v>0.02</v>
@@ -2586,7 +2586,7 @@
         <v>3.24</v>
       </c>
       <c r="B279">
-        <v>-0.06</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2599,7 +2599,7 @@
     </row>
     <row r="281" spans="1:2">
       <c r="A281">
-        <v>3</v>
+        <v>2.98</v>
       </c>
       <c r="B281">
         <v>0.01</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="282" spans="1:2">
       <c r="A282">
-        <v>2.9</v>
+        <v>2.95</v>
       </c>
       <c r="B282">
         <v>0.02</v>
@@ -2615,15 +2615,15 @@
     </row>
     <row r="283" spans="1:2">
       <c r="A283">
-        <v>2.91</v>
+        <v>2.94</v>
       </c>
       <c r="B283">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284">
-        <v>2.89</v>
+        <v>2.91</v>
       </c>
       <c r="B284">
         <v>-0.04</v>
@@ -2631,15 +2631,15 @@
     </row>
     <row r="285" spans="1:2">
       <c r="A285">
-        <v>2.9</v>
+        <v>2.91</v>
       </c>
       <c r="B285">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286">
-        <v>2.86</v>
+        <v>2.87</v>
       </c>
       <c r="B286">
         <v>-0.04</v>
@@ -2647,23 +2647,23 @@
     </row>
     <row r="287" spans="1:2">
       <c r="A287">
-        <v>2.85</v>
+        <v>2.86</v>
       </c>
       <c r="B287">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288">
-        <v>2.81</v>
+        <v>2.82</v>
       </c>
       <c r="B288">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289">
-        <v>2.85</v>
+        <v>2.87</v>
       </c>
       <c r="B289">
         <v>-0.14</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="290" spans="1:2">
       <c r="A290">
-        <v>2.82</v>
+        <v>2.83</v>
       </c>
       <c r="B290">
         <v>-0.12</v>
@@ -2679,7 +2679,7 @@
     </row>
     <row r="291" spans="1:2">
       <c r="A291">
-        <v>2.81</v>
+        <v>2.82</v>
       </c>
       <c r="B291">
         <v>-0.11</v>
@@ -2687,23 +2687,23 @@
     </row>
     <row r="292" spans="1:2">
       <c r="A292">
-        <v>2.8</v>
+        <v>2.81</v>
       </c>
       <c r="B292">
-        <v>-0.11</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293">
-        <v>2.86</v>
+        <v>2.87</v>
       </c>
       <c r="B293">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294">
-        <v>2.86</v>
+        <v>2.87</v>
       </c>
       <c r="B294">
         <v>-0.14</v>
@@ -2711,15 +2711,15 @@
     </row>
     <row r="295" spans="1:2">
       <c r="A295">
-        <v>2.89</v>
+        <v>2.92</v>
       </c>
       <c r="B295">
-        <v>-0.11</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296">
-        <v>2.95</v>
+        <v>2.96</v>
       </c>
       <c r="B296">
         <v>-0.11</v>
@@ -2727,18 +2727,18 @@
     </row>
     <row r="297" spans="1:2">
       <c r="A297">
-        <v>2.88</v>
+        <v>2.93</v>
       </c>
       <c r="B297">
-        <v>-0.07000000000000001</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298">
-        <v>2.9</v>
+        <v>2.91</v>
       </c>
       <c r="B298">
-        <v>-0.11</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2754,7 +2754,7 @@
         <v>3.05</v>
       </c>
       <c r="B300">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2767,15 +2767,15 @@
     </row>
     <row r="302" spans="1:2">
       <c r="A302">
-        <v>3.15</v>
+        <v>3.16</v>
       </c>
       <c r="B302">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="303" spans="1:2">
       <c r="A303">
-        <v>3.15</v>
+        <v>3.16</v>
       </c>
       <c r="B303">
         <v>-0.11</v>
@@ -2783,7 +2783,7 @@
     </row>
     <row r="304" spans="1:2">
       <c r="A304">
-        <v>3.29</v>
+        <v>3.3</v>
       </c>
       <c r="B304">
         <v>-0.1</v>
@@ -2791,10 +2791,10 @@
     </row>
     <row r="305" spans="1:2">
       <c r="A305">
-        <v>3.33</v>
+        <v>3.34</v>
       </c>
       <c r="B305">
-        <v>-0.08</v>
+        <v>-0.07000000000000001</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2815,15 +2815,15 @@
     </row>
     <row r="308" spans="1:2">
       <c r="A308">
-        <v>3.52</v>
+        <v>3.55</v>
       </c>
       <c r="B308">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
     </row>
     <row r="309" spans="1:2">
       <c r="A309">
-        <v>3.6</v>
+        <v>3.62</v>
       </c>
       <c r="B309">
         <v>-0.02</v>
@@ -2831,7 +2831,7 @@
     </row>
     <row r="310" spans="1:2">
       <c r="A310">
-        <v>3.7</v>
+        <v>3.71</v>
       </c>
       <c r="B310">
         <v>0.01</v>
@@ -2839,23 +2839,23 @@
     </row>
     <row r="311" spans="1:2">
       <c r="A311">
-        <v>3.71</v>
+        <v>3.74</v>
       </c>
       <c r="B311">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312">
-        <v>3.8</v>
+        <v>3.81</v>
       </c>
       <c r="B312">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313">
-        <v>3.93</v>
+        <v>3.92</v>
       </c>
       <c r="B313">
         <v>0.02</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="314" spans="1:2">
       <c r="A314">
-        <v>3.96</v>
+        <v>3.99</v>
       </c>
       <c r="B314">
         <v>0.03</v>
@@ -2879,10 +2879,10 @@
     </row>
     <row r="316" spans="1:2">
       <c r="A316">
-        <v>4.11</v>
+        <v>4.12</v>
       </c>
       <c r="B316">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2903,7 +2903,7 @@
     </row>
     <row r="319" spans="1:2">
       <c r="A319">
-        <v>4.29</v>
+        <v>4.3</v>
       </c>
       <c r="B319">
         <v>0.01</v>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="321" spans="1:2">
       <c r="A321">
-        <v>4.48</v>
+        <v>4.49</v>
       </c>
       <c r="B321">
         <v>0.03</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="322" spans="1:2">
       <c r="A322">
-        <v>4.53</v>
+        <v>4.56</v>
       </c>
       <c r="B322">
         <v>0.03</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="323" spans="1:2">
       <c r="A323">
-        <v>4.62</v>
+        <v>4.63</v>
       </c>
       <c r="B323">
         <v>0.02</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="324" spans="1:2">
       <c r="A324">
-        <v>4.63</v>
+        <v>4.65</v>
       </c>
       <c r="B324">
         <v>0.03</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="326" spans="1:2">
       <c r="A326">
-        <v>4.62</v>
+        <v>4.63</v>
       </c>
       <c r="B326">
         <v>0.03</v>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="327" spans="1:2">
       <c r="A327">
-        <v>4.67</v>
+        <v>4.69</v>
       </c>
       <c r="B327">
         <v>0.02</v>
@@ -2975,7 +2975,7 @@
     </row>
     <row r="328" spans="1:2">
       <c r="A328">
-        <v>4.75</v>
+        <v>4.77</v>
       </c>
       <c r="B328">
         <v>0</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="329" spans="1:2">
       <c r="A329">
-        <v>4.76</v>
+        <v>4.77</v>
       </c>
       <c r="B329">
         <v>-0.01</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="330" spans="1:2">
       <c r="A330">
-        <v>4.75</v>
+        <v>4.76</v>
       </c>
       <c r="B330">
         <v>0.04</v>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="331" spans="1:2">
       <c r="A331">
-        <v>4.68</v>
+        <v>4.71</v>
       </c>
       <c r="B331">
         <v>0.04</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="332" spans="1:2">
       <c r="A332">
-        <v>4.66</v>
+        <v>4.68</v>
       </c>
       <c r="B332">
         <v>0.02</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="333" spans="1:2">
       <c r="A333">
-        <v>4.71</v>
+        <v>4.73</v>
       </c>
       <c r="B333">
         <v>-0.03</v>

</xml_diff>